<commit_message>
2-ch single ended working.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -706,7 +706,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>0x0F</v>
+        <v>0x03</v>
       </c>
       <c r="D14" s="11">
         <v>0</v>
@@ -1287,10 +1287,10 @@
         <v>0</v>
       </c>
       <c r="H14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="4">
         <v>1</v>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>0x00</v>
+        <v>0x03</v>
       </c>
       <c r="D15" s="11">
         <v>0</v>
@@ -1335,10 +1335,10 @@
         <v>0</v>
       </c>
       <c r="J15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="4">
         <v>51</v>

</xml_diff>